<commit_message>
convert git page to RMD file and add download links
</commit_message>
<xml_diff>
--- a/basinCharacteristics/Covariate Data Status - High Res Delineation.xlsx
+++ b/basinCharacteristics/Covariate Data Status - High Res Delineation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="322">
   <si>
     <t>forest</t>
   </si>
@@ -930,39 +930,6 @@
     <t>1:24k polygons</t>
   </si>
   <si>
-    <t>30m</t>
-  </si>
-  <si>
-    <t>~2.3km</t>
-  </si>
-  <si>
-    <t>800m</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,360</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,361</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,362</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,363</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,364</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,365</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,366</t>
-  </si>
-  <si>
-    <t>1:12,000 to 1:63,367</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -1216,6 +1183,18 @@
   </si>
   <si>
     <t>The percentage of the catchment area that is covered by wetlands, lakes, or ponds that intersect the high resolution stream network.</t>
+  </si>
+  <si>
+    <t>30m grid cell</t>
+  </si>
+  <si>
+    <t>~2.3km grid cell</t>
+  </si>
+  <si>
+    <t>800m grid cell</t>
+  </si>
+  <si>
+    <t>1:12,000 to 1:63,360 polygons</t>
   </si>
 </sst>
 </file>
@@ -2721,10 +2700,10 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -2760,7 +2739,7 @@
         <v>49</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>48</v>
@@ -2813,13 +2792,13 @@
         <v>178</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>196</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>181</v>
@@ -2828,7 +2807,7 @@
         <v>232</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>46</v>
@@ -2873,13 +2852,13 @@
         <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>181</v>
@@ -2888,7 +2867,7 @@
         <v>232</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>46</v>
@@ -2933,13 +2912,13 @@
         <v>179</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>197</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>181</v>
@@ -2948,7 +2927,7 @@
         <v>232</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>46</v>
@@ -2993,13 +2972,13 @@
         <v>177</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>181</v>
@@ -3008,7 +2987,7 @@
         <v>232</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>46</v>
@@ -3053,13 +3032,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>181</v>
@@ -3068,7 +3047,7 @@
         <v>232</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>46</v>
@@ -3113,13 +3092,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>181</v>
@@ -3128,7 +3107,7 @@
         <v>232</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>46</v>
@@ -3179,13 +3158,13 @@
         <v>50</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>68</v>
@@ -3233,22 +3212,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>137</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>182</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>234</v>
+        <v>319</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>14</v>
@@ -3293,22 +3272,22 @@
         <v>12</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>138</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>182</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>234</v>
+        <v>319</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>14</v>
@@ -3353,22 +3332,22 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>170</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>171</v>
@@ -3413,22 +3392,22 @@
         <v>134</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>136</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>9</v>
@@ -3479,16 +3458,16 @@
         <v>103</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>183</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>9</v>
@@ -3533,22 +3512,22 @@
         <v>89</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C14" s="41" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>46</v>
@@ -3593,22 +3572,22 @@
         <v>43</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>46</v>
@@ -3653,22 +3632,22 @@
         <v>75</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C16" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>46</v>
@@ -3713,22 +3692,22 @@
         <v>39</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>86</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>46</v>
@@ -3773,22 +3752,22 @@
         <v>41</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>84</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>46</v>
@@ -3833,22 +3812,22 @@
         <v>40</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>46</v>
@@ -3893,22 +3872,22 @@
         <v>42</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>83</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>46</v>
@@ -3953,22 +3932,22 @@
         <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>79</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>46</v>
@@ -4013,22 +3992,22 @@
         <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>46</v>
@@ -4073,22 +4052,22 @@
         <v>90</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>91</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>46</v>
@@ -4132,22 +4111,22 @@
         <v>45</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>46</v>
@@ -4191,22 +4170,22 @@
         <v>5</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>46</v>
@@ -4250,22 +4229,22 @@
         <v>3</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>81</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>46</v>
@@ -4310,22 +4289,22 @@
         <v>4</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>87</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>184</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>233</v>
+        <v>318</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>46</v>
@@ -4369,22 +4348,22 @@
         <v>215</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>217</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>233</v>
+      <c r="F28" s="9" t="s">
+        <v>318</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="H28" s="32" t="s">
         <v>9</v>
@@ -4429,22 +4408,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>10</v>
@@ -4489,22 +4468,22 @@
         <v>32</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>129</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>10</v>
@@ -4549,22 +4528,22 @@
         <v>36</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>133</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>10</v>
@@ -4609,22 +4588,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>123</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>10</v>
@@ -4669,22 +4648,22 @@
         <v>25</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>122</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>10</v>
@@ -4729,22 +4708,22 @@
         <v>31</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>10</v>
@@ -4789,22 +4768,22 @@
         <v>30</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>10</v>
@@ -4849,22 +4828,22 @@
         <v>27</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>124</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>10</v>
@@ -4909,22 +4888,22 @@
         <v>6</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>120</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>135</v>
@@ -4969,22 +4948,22 @@
         <v>29</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>126</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>10</v>
@@ -5029,22 +5008,22 @@
         <v>7</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>121</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>135</v>
@@ -5089,22 +5068,22 @@
         <v>35</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>10</v>
@@ -5149,22 +5128,22 @@
         <v>34</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>131</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>10</v>
@@ -5209,22 +5188,22 @@
         <v>33</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>130</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>146</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>10</v>
@@ -5269,22 +5248,22 @@
         <v>206</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C43" s="39" t="s">
         <v>214</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F43" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H43" s="32" t="s">
         <v>218</v>
@@ -5329,22 +5308,22 @@
         <v>199</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C44" s="39" t="s">
         <v>207</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F44" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H44" s="32" t="s">
         <v>218</v>
@@ -5389,22 +5368,22 @@
         <v>200</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C45" s="39" t="s">
         <v>208</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F45" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H45" s="32" t="s">
         <v>218</v>
@@ -5449,22 +5428,22 @@
         <v>201</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C46" s="39" t="s">
         <v>209</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H46" s="32" t="s">
         <v>218</v>
@@ -5509,22 +5488,22 @@
         <v>202</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C47" s="39" t="s">
         <v>210</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F47" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H47" s="32" t="s">
         <v>218</v>
@@ -5569,22 +5548,22 @@
         <v>203</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C48" s="39" t="s">
         <v>211</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H48" s="32" t="s">
         <v>218</v>
@@ -5629,22 +5608,22 @@
         <v>204</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C49" s="39" t="s">
         <v>212</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F49" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H49" s="32" t="s">
         <v>218</v>
@@ -5689,22 +5668,22 @@
         <v>205</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>213</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>219</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="H50" s="32" t="s">
         <v>218</v>
@@ -5749,22 +5728,22 @@
         <v>102</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>106</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E51" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>242</v>
+        <v>321</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>46</v>
@@ -5809,22 +5788,22 @@
         <v>18</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E52" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>114</v>
@@ -5869,22 +5848,22 @@
         <v>19</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>108</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E53" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>46</v>
@@ -5929,22 +5908,22 @@
         <v>20</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>109</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E54" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>238</v>
+        <v>321</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>46</v>
@@ -5989,22 +5968,22 @@
         <v>21</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>110</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E55" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>239</v>
+        <v>321</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>46</v>
@@ -6049,22 +6028,22 @@
         <v>23</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E56" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>241</v>
+        <v>321</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H56" s="13" t="s">
         <v>46</v>
@@ -6109,22 +6088,22 @@
         <v>22</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>111</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E57" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>240</v>
+        <v>321</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H57" s="13" t="s">
         <v>46</v>
@@ -6169,22 +6148,22 @@
         <v>8</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E58" s="36" t="s">
         <v>185</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>243</v>
+        <v>321</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>46</v>
@@ -6273,7 +6252,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>66</v>
@@ -6431,10 +6410,10 @@
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>220</v>
@@ -6443,25 +6422,25 @@
         <v>37</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F11" s="1"/>
     </row>

</xml_diff>